<commit_message>
version 1.1(all test cases had added)
</commit_message>
<xml_diff>
--- a/data/testcases.xlsx
+++ b/data/testcases.xlsx
@@ -1,31 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="3" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="7935" windowWidth="20400"/>
+    <workbookView activeTab="3" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="7935" windowWidth="20400" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sendMCode" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="userRegister" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="verifyUserAuth" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="bindBankCard" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="sendMCode" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="userRegister" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="verifyUserAuth" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="bindBankCard" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="144525" fullCalcOnLoad="1"/>
+  <calcPr calcId="125725" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ " numFmtId="164"/>
-    <numFmt formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ " numFmtId="165"/>
-    <numFmt formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ " numFmtId="166"/>
-    <numFmt formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ " numFmtId="167"/>
-  </numFmts>
-  <fonts count="29">
+  <numFmts count="0"/>
+  <fonts count="14">
     <font>
       <name val="宋体"/>
       <charset val="134"/>
@@ -55,7 +50,7 @@
     </font>
     <font>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <color theme="1"/>
       <sz val="10.5"/>
     </font>
@@ -77,146 +72,29 @@
     </font>
     <font>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <b val="1"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <color theme="0"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <b val="1"/>
-      <color rgb="FFFA7D00"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <name val="宋体"/>
       <charset val="134"/>
       <b val="1"/>
-      <color theme="3"/>
-      <sz val="13"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <color theme="1"/>
+      <color rgb="FF00FF00"/>
       <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <color rgb="FF006100"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <b val="1"/>
-      <color rgb="FF3F3F3F"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <color rgb="FF0000FF"/>
-      <sz val="11"/>
-      <u val="single"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <color rgb="FF9C0006"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <i val="1"/>
-      <color rgb="FF7F7F7F"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <color rgb="FFFA7D00"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <name val="宋体"/>
       <charset val="134"/>
       <b val="1"/>
-      <color theme="3"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
       <color rgb="FFFF0000"/>
       <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <color rgb="FF3F3F76"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <name val="宋体"/>
       <charset val="134"/>
-      <b val="1"/>
-      <color theme="3"/>
-      <sz val="15"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <b val="1"/>
-      <color rgb="FFFFFFFF"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <color rgb="FF9C6500"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <b val="1"/>
-      <color theme="3"/>
-      <sz val="18"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <color rgb="FF800080"/>
-      <sz val="11"/>
-      <u val="single"/>
+      <sz val="9"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -232,7 +110,7 @@
       <color rgb="00FF0000"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -247,192 +125,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="17">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -528,104 +226,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
@@ -635,156 +235,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="12" fontId="11" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="9" fillId="18" fontId="20" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="165">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="166">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="5" fontId="11" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="8" fontId="15" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="167">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="17" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="14" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="25" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="12" fillId="11" fontId="0" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="27" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="18" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="19" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="24" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="16" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="10" fillId="0" fontId="21" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="10" fillId="0" fontId="10" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="16" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="14" fillId="0" fontId="18" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="14" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="11" fillId="4" fontId="13" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="9" fillId="4" fontId="9" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="15" fillId="24" fontId="22" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="28" fontId="11" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="3" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="13" fillId="0" fontId="17" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="8" fillId="0" fontId="7" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="7" fontId="12" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="26" fontId="23" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="23" fontId="11" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="10" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="9" fontId="11" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="21" fontId="11" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="13" fontId="11" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="6" fontId="11" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="20" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="22" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="25" fontId="11" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="15" fontId="11" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="19" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="30" fontId="11" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="31" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="33" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="29" fontId="11" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="32" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="45">
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -832,13 +288,7 @@
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="4" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf applyAlignment="1" borderId="5" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="6" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf applyAlignment="1" borderId="7" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
@@ -847,70 +297,50 @@
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="26" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="27" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="28" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="9" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="26" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="28" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="0" fontId="26" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="0" fontId="27" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="3" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="4" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="6" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="11" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="12" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="11" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="0" fontId="12" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="13" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle builtinId="0" name="常规" xfId="0"/>
-    <cellStyle builtinId="7" name="货币[0]" xfId="1"/>
-    <cellStyle builtinId="38" name="20% - 强调文字颜色 3" xfId="2"/>
-    <cellStyle builtinId="20" name="输入" xfId="3"/>
-    <cellStyle builtinId="4" name="货币" xfId="4"/>
-    <cellStyle builtinId="6" name="千位分隔[0]" xfId="5"/>
-    <cellStyle builtinId="39" name="40% - 强调文字颜色 3" xfId="6"/>
-    <cellStyle builtinId="27" name="差" xfId="7"/>
-    <cellStyle builtinId="3" name="千位分隔" xfId="8"/>
-    <cellStyle builtinId="40" name="60% - 强调文字颜色 3" xfId="9"/>
-    <cellStyle builtinId="8" name="超链接" xfId="10"/>
-    <cellStyle builtinId="5" name="百分比" xfId="11"/>
-    <cellStyle builtinId="9" name="已访问的超链接" xfId="12"/>
-    <cellStyle builtinId="10" name="注释" xfId="13"/>
-    <cellStyle builtinId="36" name="60% - 强调文字颜色 2" xfId="14"/>
-    <cellStyle builtinId="19" name="标题 4" xfId="15"/>
-    <cellStyle builtinId="11" name="警告文本" xfId="16"/>
-    <cellStyle builtinId="15" name="标题" xfId="17"/>
-    <cellStyle builtinId="53" name="解释性文本" xfId="18"/>
-    <cellStyle builtinId="16" name="标题 1" xfId="19"/>
-    <cellStyle builtinId="17" name="标题 2" xfId="20"/>
-    <cellStyle builtinId="32" name="60% - 强调文字颜色 1" xfId="21"/>
-    <cellStyle builtinId="18" name="标题 3" xfId="22"/>
-    <cellStyle builtinId="44" name="60% - 强调文字颜色 4" xfId="23"/>
-    <cellStyle builtinId="21" name="输出" xfId="24"/>
-    <cellStyle builtinId="22" name="计算" xfId="25"/>
-    <cellStyle builtinId="23" name="检查单元格" xfId="26"/>
-    <cellStyle builtinId="50" name="20% - 强调文字颜色 6" xfId="27"/>
-    <cellStyle builtinId="33" name="强调文字颜色 2" xfId="28"/>
-    <cellStyle builtinId="24" name="链接单元格" xfId="29"/>
-    <cellStyle builtinId="25" name="汇总" xfId="30"/>
-    <cellStyle builtinId="26" name="好" xfId="31"/>
-    <cellStyle builtinId="28" name="适中" xfId="32"/>
-    <cellStyle builtinId="46" name="20% - 强调文字颜色 5" xfId="33"/>
-    <cellStyle builtinId="29" name="强调文字颜色 1" xfId="34"/>
-    <cellStyle builtinId="30" name="20% - 强调文字颜色 1" xfId="35"/>
-    <cellStyle builtinId="31" name="40% - 强调文字颜色 1" xfId="36"/>
-    <cellStyle builtinId="34" name="20% - 强调文字颜色 2" xfId="37"/>
-    <cellStyle builtinId="35" name="40% - 强调文字颜色 2" xfId="38"/>
-    <cellStyle builtinId="37" name="强调文字颜色 3" xfId="39"/>
-    <cellStyle builtinId="41" name="强调文字颜色 4" xfId="40"/>
-    <cellStyle builtinId="42" name="20% - 强调文字颜色 4" xfId="41"/>
-    <cellStyle builtinId="43" name="40% - 强调文字颜色 4" xfId="42"/>
-    <cellStyle builtinId="45" name="强调文字颜色 5" xfId="43"/>
-    <cellStyle builtinId="47" name="40% - 强调文字颜色 5" xfId="44"/>
-    <cellStyle builtinId="48" name="60% - 强调文字颜色 5" xfId="45"/>
-    <cellStyle builtinId="49" name="强调文字颜色 6" xfId="46"/>
-    <cellStyle builtinId="51" name="40% - 强调文字颜色 6" xfId="47"/>
-    <cellStyle builtinId="52" name="60% - 强调文字颜色 6" xfId="48"/>
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
@@ -1197,6 +627,7 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
@@ -1209,73 +640,73 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" max="2" min="2" style="1" width="12.25"/>
-    <col customWidth="1" max="3" min="3" style="1" width="25.625"/>
-    <col customWidth="1" max="4" min="4" style="1" width="38.5"/>
-    <col customWidth="1" max="5" min="5" style="1" width="62.25"/>
-    <col customWidth="1" max="6" min="6" style="1" width="10.625"/>
-    <col customWidth="1" max="7" min="7" style="1" width="49"/>
-    <col customWidth="1" max="8" min="8" style="1" width="72"/>
-    <col customWidth="1" max="9" min="9" style="1" width="5.875"/>
+    <col customWidth="1" max="2" min="2" style="36" width="12.25"/>
+    <col customWidth="1" max="3" min="3" style="36" width="25.625"/>
+    <col customWidth="1" max="4" min="4" style="36" width="38.5"/>
+    <col customWidth="1" max="5" min="5" style="36" width="62.25"/>
+    <col customWidth="1" max="6" min="6" style="36" width="10.625"/>
+    <col customWidth="1" max="7" min="7" style="36" width="49"/>
+    <col customWidth="1" max="8" min="8" style="36" width="72"/>
+    <col customWidth="1" max="9" min="9" style="36" width="5.875"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="7" t="inlineStr">
+      <c r="A1" s="37" t="inlineStr">
         <is>
           <t>CaseId</t>
         </is>
       </c>
-      <c r="B1" s="7" t="inlineStr">
+      <c r="B1" s="37" t="inlineStr">
         <is>
           <t>Precondition</t>
         </is>
       </c>
-      <c r="C1" s="7" t="inlineStr">
+      <c r="C1" s="37" t="inlineStr">
         <is>
           <t>Title</t>
         </is>
       </c>
-      <c r="D1" s="7" t="inlineStr">
+      <c r="D1" s="37" t="inlineStr">
         <is>
           <t>URL</t>
         </is>
       </c>
-      <c r="E1" s="7" t="inlineStr">
+      <c r="E1" s="37" t="inlineStr">
         <is>
           <t>Data</t>
         </is>
       </c>
-      <c r="F1" s="7" t="inlineStr">
+      <c r="F1" s="37" t="inlineStr">
         <is>
           <t>ApiName</t>
         </is>
       </c>
-      <c r="G1" s="7" t="inlineStr">
+      <c r="G1" s="37" t="inlineStr">
         <is>
           <t>Expected</t>
         </is>
       </c>
-      <c r="H1" s="7" t="inlineStr">
+      <c r="H1" s="37" t="inlineStr">
         <is>
           <t>Actual</t>
         </is>
       </c>
-      <c r="I1" s="7" t="inlineStr">
+      <c r="I1" s="37" t="inlineStr">
         <is>
           <t>Result</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="n">
+      <c r="A2" s="31" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="inlineStr">
+      <c r="B2" s="31" t="inlineStr">
         <is>
           <t>无</t>
         </is>
@@ -1305,22 +736,22 @@
           <t>{"retCode": "0", "retInfo": "ok"}</t>
         </is>
       </c>
-      <c r="H2" s="26" t="inlineStr">
+      <c r="H2" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 0, 'retInfo': ok}</t>
         </is>
       </c>
-      <c r="I2" s="27" t="inlineStr">
+      <c r="I2" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="n">
+      <c r="A3" s="31" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="11" t="n"/>
+      <c r="B3" s="32" t="n"/>
       <c r="C3" s="7" t="inlineStr">
         <is>
           <t>发送成功-IP地址非String类型</t>
@@ -1346,22 +777,22 @@
           <t>{"retCode": "0", "retInfo": "ok"}</t>
         </is>
       </c>
-      <c r="H3" s="26" t="inlineStr">
+      <c r="H3" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 0, 'retInfo': ok}</t>
         </is>
       </c>
-      <c r="I3" s="27" t="inlineStr">
+      <c r="I3" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="n">
+      <c r="A4" s="31" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="11" t="n"/>
+      <c r="B4" s="32" t="n"/>
       <c r="C4" s="7" t="inlineStr">
         <is>
           <t>发送失败-IP地址为空</t>
@@ -1387,22 +818,22 @@
           <t>{"faultcode": "soap:Server", "faultstring": "用户IP不能为空"}</t>
         </is>
       </c>
-      <c r="H4" s="26" t="inlineStr">
+      <c r="H4" s="38" t="inlineStr">
         <is>
           <t>{'faultcode': soap:Server, 'faultstring': 用户IP不能为空}</t>
         </is>
       </c>
-      <c r="I4" s="27" t="inlineStr">
+      <c r="I4" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="n">
+      <c r="A5" s="31" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="11" t="n"/>
+      <c r="B5" s="32" t="n"/>
       <c r="C5" s="7" t="inlineStr">
         <is>
           <t>发送失败-IP地址参数缺失</t>
@@ -1428,22 +859,22 @@
           <t>{"faultcode": "soap:Server", "faultstring": "用户IP不能为空"}</t>
         </is>
       </c>
-      <c r="H5" s="26" t="inlineStr">
+      <c r="H5" s="38" t="inlineStr">
         <is>
           <t>{'faultcode': soap:Server, 'faultstring': 用户IP不能为空}</t>
         </is>
       </c>
-      <c r="I5" s="27" t="inlineStr">
+      <c r="I5" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="5" t="n">
+      <c r="A6" s="31" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="11" t="n"/>
+      <c r="B6" s="32" t="n"/>
       <c r="C6" s="7" t="inlineStr">
         <is>
           <t>发送失败-短信模板参数缺失</t>
@@ -1469,22 +900,22 @@
           <t>{"faultcode": "soap:Server", "faultstring": "短信模板ID错误"}</t>
         </is>
       </c>
-      <c r="H6" s="26" t="inlineStr">
+      <c r="H6" s="38" t="inlineStr">
         <is>
           <t>{'faultcode': soap:Server, 'faultstring': 短信模板ID错误}</t>
         </is>
       </c>
-      <c r="I6" s="27" t="inlineStr">
+      <c r="I6" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="5" t="n">
+      <c r="A7" s="31" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="11" t="n"/>
+      <c r="B7" s="32" t="n"/>
       <c r="C7" s="7" t="inlineStr">
         <is>
           <t>发送失败-手机号码参数缺失</t>
@@ -1510,22 +941,22 @@
           <t>{"faultcode": "soap:Server", "faultstring": "手机号码错误"}</t>
         </is>
       </c>
-      <c r="H7" s="26" t="inlineStr">
+      <c r="H7" s="38" t="inlineStr">
         <is>
           <t>{'faultcode': soap:Server, 'faultstring': 手机号码错误}</t>
         </is>
       </c>
-      <c r="I7" s="27" t="inlineStr">
+      <c r="I7" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="5" t="n">
+      <c r="A8" s="31" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="11" t="n"/>
+      <c r="B8" s="32" t="n"/>
       <c r="C8" s="7" t="inlineStr">
         <is>
           <t>发送失败-手机号码为空</t>
@@ -1551,22 +982,22 @@
           <t>{"faultcode": "soap:Server", "faultstring": "手机号码错误"}</t>
         </is>
       </c>
-      <c r="H8" s="26" t="inlineStr">
+      <c r="H8" s="38" t="inlineStr">
         <is>
           <t>{'faultcode': soap:Server, 'faultstring': 手机号码错误}</t>
         </is>
       </c>
-      <c r="I8" s="27" t="inlineStr">
+      <c r="I8" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="5" t="n">
+      <c r="A9" s="31" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="11" t="n"/>
+      <c r="B9" s="32" t="n"/>
       <c r="C9" s="7" t="inlineStr">
         <is>
           <t>发送失败-手机号码非11位</t>
@@ -1592,22 +1023,22 @@
           <t>{"faultcode": "soap:Server", "faultstring": "手机号码错误"}</t>
         </is>
       </c>
-      <c r="H9" s="26" t="inlineStr">
+      <c r="H9" s="38" t="inlineStr">
         <is>
           <t>{'faultcode': soap:Server, 'faultstring': 手机号码错误}</t>
         </is>
       </c>
-      <c r="I9" s="27" t="inlineStr">
+      <c r="I9" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="5" t="n">
+      <c r="A10" s="31" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="11" t="n"/>
+      <c r="B10" s="32" t="n"/>
       <c r="C10" s="7" t="inlineStr">
         <is>
           <t>发送失败-短信模板为空</t>
@@ -1633,22 +1064,22 @@
           <t>{"faultcode": "soap:Server", "faultstring": "短信模板ID错误"}</t>
         </is>
       </c>
-      <c r="H10" s="26" t="inlineStr">
+      <c r="H10" s="38" t="inlineStr">
         <is>
           <t>{'faultcode': soap:Server, 'faultstring': 短信模板ID错误}</t>
         </is>
       </c>
-      <c r="I10" s="27" t="inlineStr">
+      <c r="I10" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="5" t="n">
+      <c r="A11" s="31" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="11" t="n"/>
+      <c r="B11" s="32" t="n"/>
       <c r="C11" s="7" t="inlineStr">
         <is>
           <t>发送失败-短信模板不为1</t>
@@ -1674,22 +1105,22 @@
           <t>{"faultcode": "soap:Server", "faultstring": "短信模板配置错误"}</t>
         </is>
       </c>
-      <c r="H11" s="26" t="inlineStr">
+      <c r="H11" s="38" t="inlineStr">
         <is>
           <t>{'faultcode': soap:Server, 'faultstring': 短信模板配置错误}</t>
         </is>
       </c>
-      <c r="I11" s="27" t="inlineStr">
+      <c r="I11" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="5" t="n">
+      <c r="A12" s="31" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="11" t="n"/>
+      <c r="B12" s="32" t="n"/>
       <c r="C12" s="7" t="inlineStr">
         <is>
           <t>发送成功-短信模板非String类型</t>
@@ -1715,22 +1146,22 @@
           <t>{"faultcode": "soap:Server", "faultstring": "短信模板配置错误"}</t>
         </is>
       </c>
-      <c r="H12" s="26" t="inlineStr">
+      <c r="H12" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 0, 'retInfo': ok}</t>
         </is>
       </c>
-      <c r="I12" s="28" t="inlineStr">
+      <c r="I12" s="42" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="5" t="n">
+      <c r="A13" s="31" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="12" t="n"/>
+      <c r="B13" s="33" t="n"/>
       <c r="C13" s="7" t="inlineStr">
         <is>
           <t>发送失败-手机号码非String类型</t>
@@ -1756,12 +1187,12 @@
           <t>{"faultcode": "soap:Server", "faultstring": "手机号码错误"}</t>
         </is>
       </c>
-      <c r="H13" s="26" t="inlineStr">
+      <c r="H13" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 0, 'retInfo': ok}</t>
         </is>
       </c>
-      <c r="I13" s="28" t="inlineStr">
+      <c r="I13" s="42" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
@@ -1783,81 +1214,81 @@
   </sheetPr>
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="1" width="9.125"/>
-    <col customWidth="1" max="2" min="2" style="1" width="35.375"/>
-    <col customWidth="1" max="3" min="3" style="1" width="38.75"/>
-    <col customWidth="1" max="4" min="4" style="1" width="52.625"/>
-    <col customWidth="1" max="5" min="5" style="1" width="132"/>
-    <col customWidth="1" max="6" min="6" style="1" width="10.75"/>
-    <col customWidth="1" max="7" min="7" style="1" width="80.625"/>
-    <col customWidth="1" max="8" min="8" style="1" width="81"/>
-    <col customWidth="1" max="9" min="9" style="1" width="5.875"/>
-    <col customWidth="1" max="10" min="10" style="1" width="90.75"/>
+    <col customWidth="1" max="1" min="1" style="36" width="9.125"/>
+    <col customWidth="1" max="2" min="2" style="36" width="35.375"/>
+    <col customWidth="1" max="3" min="3" style="36" width="38.75"/>
+    <col customWidth="1" max="4" min="4" style="36" width="52.625"/>
+    <col customWidth="1" max="5" min="5" style="36" width="132"/>
+    <col customWidth="1" max="6" min="6" style="36" width="10.75"/>
+    <col customWidth="1" max="7" min="7" style="36" width="80.625"/>
+    <col customWidth="1" max="8" min="8" style="36" width="81"/>
+    <col customWidth="1" max="9" min="9" style="36" width="5.875"/>
+    <col customWidth="1" max="10" min="10" style="36" width="90.75"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="7" t="inlineStr">
+      <c r="A1" s="37" t="inlineStr">
         <is>
           <t>CaseId</t>
         </is>
       </c>
-      <c r="B1" s="7" t="inlineStr">
+      <c r="B1" s="37" t="inlineStr">
         <is>
           <t>Precondition</t>
         </is>
       </c>
-      <c r="C1" s="7" t="inlineStr">
+      <c r="C1" s="37" t="inlineStr">
         <is>
           <t>Title</t>
         </is>
       </c>
-      <c r="D1" s="7" t="inlineStr">
+      <c r="D1" s="37" t="inlineStr">
         <is>
           <t>URL</t>
         </is>
       </c>
-      <c r="E1" s="7" t="inlineStr">
+      <c r="E1" s="37" t="inlineStr">
         <is>
           <t>Data</t>
         </is>
       </c>
-      <c r="F1" s="7" t="inlineStr">
+      <c r="F1" s="37" t="inlineStr">
         <is>
           <t>ApiName</t>
         </is>
       </c>
-      <c r="G1" s="7" t="inlineStr">
+      <c r="G1" s="37" t="inlineStr">
         <is>
           <t>Expected</t>
         </is>
       </c>
-      <c r="H1" s="7" t="inlineStr">
+      <c r="H1" s="37" t="inlineStr">
         <is>
           <t>Actual</t>
         </is>
       </c>
-      <c r="I1" s="7" t="inlineStr">
+      <c r="I1" s="37" t="inlineStr">
         <is>
           <t>Result</t>
         </is>
       </c>
-      <c r="J1" s="7" t="inlineStr">
+      <c r="J1" s="37" t="inlineStr">
         <is>
           <t>Sql</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="27" r="2" s="1">
-      <c r="A2" s="5" t="n">
+    <row customHeight="1" ht="27" r="2" s="36">
+      <c r="A2" s="31" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="25" t="inlineStr">
+      <c r="B2" s="23" t="inlineStr">
         <is>
           <t>注册的手机号与接收验证码的手机号相同且验证码有效</t>
         </is>
@@ -1887,12 +1318,12 @@
           <t>{"retCode": "0", "retInfo": "ok"}</t>
         </is>
       </c>
-      <c r="H2" s="26" t="inlineStr">
+      <c r="H2" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 0, 'retInfo': ok}</t>
         </is>
       </c>
-      <c r="I2" s="27" t="inlineStr">
+      <c r="I2" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
@@ -1904,7 +1335,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="n">
+      <c r="A3" s="31" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="6" t="n"/>
@@ -1933,12 +1364,12 @@
           <t>{"retCode": "19001", "retInfo": "验证码错误"}</t>
         </is>
       </c>
-      <c r="H3" s="26" t="inlineStr">
+      <c r="H3" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 19001, 'retInfo': 验证码错误}</t>
         </is>
       </c>
-      <c r="I3" s="27" t="inlineStr">
+      <c r="I3" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
@@ -1946,7 +1377,7 @@
       <c r="J3" s="7" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="n">
+      <c r="A4" s="31" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="6" t="n"/>
@@ -1975,12 +1406,12 @@
           <t>{"retCode": "19001", "retInfo": "用户名错误"}</t>
         </is>
       </c>
-      <c r="H4" s="26" t="inlineStr">
+      <c r="H4" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 19001, 'retInfo': 用户名错误}</t>
         </is>
       </c>
-      <c r="I4" s="27" t="inlineStr">
+      <c r="I4" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
@@ -1988,7 +1419,7 @@
       <c r="J4" s="7" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="n">
+      <c r="A5" s="31" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="6" t="n"/>
@@ -2017,12 +1448,12 @@
           <t>{"retCode": "19001", "retInfo": "渠道信息错误"}</t>
         </is>
       </c>
-      <c r="H5" s="26" t="inlineStr">
+      <c r="H5" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 19001, 'retInfo': 渠道信息错误}</t>
         </is>
       </c>
-      <c r="I5" s="27" t="inlineStr">
+      <c r="I5" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
@@ -2030,7 +1461,7 @@
       <c r="J5" s="7" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="5" t="n">
+      <c r="A6" s="31" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="6" t="n"/>
@@ -2059,12 +1490,12 @@
           <t>{"retCode": "19001", "retInfo": "用户UID错误"}</t>
         </is>
       </c>
-      <c r="H6" s="26" t="inlineStr">
+      <c r="H6" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 19001, 'retInfo': 用户UID错误}</t>
         </is>
       </c>
-      <c r="I6" s="27" t="inlineStr">
+      <c r="I6" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
@@ -2072,7 +1503,7 @@
       <c r="J6" s="7" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" s="5" t="n">
+      <c r="A7" s="31" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="6" t="n"/>
@@ -2101,12 +1532,12 @@
           <t>{"retCode": "19001", "retInfo": "手机号错误"}</t>
         </is>
       </c>
-      <c r="H7" s="26" t="inlineStr">
+      <c r="H7" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 19001, 'retInfo': 手机号错误}</t>
         </is>
       </c>
-      <c r="I7" s="27" t="inlineStr">
+      <c r="I7" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
@@ -2114,7 +1545,7 @@
       <c r="J7" s="7" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="5" t="n">
+      <c r="A8" s="31" t="n">
         <v>7</v>
       </c>
       <c r="B8" s="6" t="n"/>
@@ -2143,12 +1574,12 @@
           <t>{"retCode": "19001", "retInfo": "IP地址错误"}</t>
         </is>
       </c>
-      <c r="H8" s="26" t="inlineStr">
+      <c r="H8" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 19001, 'retInfo': IP地址错误}</t>
         </is>
       </c>
-      <c r="I8" s="27" t="inlineStr">
+      <c r="I8" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
@@ -2156,7 +1587,7 @@
       <c r="J8" s="7" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="5" t="n">
+      <c r="A9" s="31" t="n">
         <v>8</v>
       </c>
       <c r="B9" s="6" t="n"/>
@@ -2185,12 +1616,12 @@
           <t>{"retCode": "19001", "retInfo": "验证码错误"}</t>
         </is>
       </c>
-      <c r="H9" s="26" t="inlineStr">
+      <c r="H9" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 19001, 'retInfo': 验证码错误}</t>
         </is>
       </c>
-      <c r="I9" s="27" t="inlineStr">
+      <c r="I9" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
@@ -2198,7 +1629,7 @@
       <c r="J9" s="7" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" s="5" t="n">
+      <c r="A10" s="31" t="n">
         <v>9</v>
       </c>
       <c r="B10" s="6" t="n"/>
@@ -2227,12 +1658,12 @@
           <t>{"retCode": "19001", "retInfo": "用户名错误"}</t>
         </is>
       </c>
-      <c r="H10" s="26" t="inlineStr">
+      <c r="H10" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 19001, 'retInfo': 用户名错误}</t>
         </is>
       </c>
-      <c r="I10" s="27" t="inlineStr">
+      <c r="I10" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
@@ -2240,7 +1671,7 @@
       <c r="J10" s="7" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="5" t="n">
+      <c r="A11" s="31" t="n">
         <v>10</v>
       </c>
       <c r="B11" s="6" t="n"/>
@@ -2269,12 +1700,12 @@
           <t>{"retCode": "19001", "retInfo": "渠道信息错误"}</t>
         </is>
       </c>
-      <c r="H11" s="26" t="inlineStr">
+      <c r="H11" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 19001, 'retInfo': 渠道信息错误}</t>
         </is>
       </c>
-      <c r="I11" s="27" t="inlineStr">
+      <c r="I11" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
@@ -2282,7 +1713,7 @@
       <c r="J11" s="7" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" s="5" t="n">
+      <c r="A12" s="31" t="n">
         <v>11</v>
       </c>
       <c r="B12" s="6" t="n"/>
@@ -2311,12 +1742,12 @@
           <t>{"retCode": "19001", "retInfo": "用户UID错误"}</t>
         </is>
       </c>
-      <c r="H12" s="26" t="inlineStr">
+      <c r="H12" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 19001, 'retInfo': 用户UID错误}</t>
         </is>
       </c>
-      <c r="I12" s="27" t="inlineStr">
+      <c r="I12" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
@@ -2324,7 +1755,7 @@
       <c r="J12" s="7" t="n"/>
     </row>
     <row r="13">
-      <c r="A13" s="5" t="n">
+      <c r="A13" s="31" t="n">
         <v>12</v>
       </c>
       <c r="B13" s="6" t="n"/>
@@ -2353,12 +1784,12 @@
           <t>{"retCode": "19001", "retInfo": "手机号错误"}</t>
         </is>
       </c>
-      <c r="H13" s="26" t="inlineStr">
+      <c r="H13" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 19001, 'retInfo': 手机号错误}</t>
         </is>
       </c>
-      <c r="I13" s="27" t="inlineStr">
+      <c r="I13" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
@@ -2366,7 +1797,7 @@
       <c r="J13" s="7" t="n"/>
     </row>
     <row r="14">
-      <c r="A14" s="5" t="n">
+      <c r="A14" s="31" t="n">
         <v>13</v>
       </c>
       <c r="B14" s="6" t="n"/>
@@ -2395,12 +1826,12 @@
           <t>{"retCode": "30010008", "retInfo": "验证码错误"}</t>
         </is>
       </c>
-      <c r="H14" s="26" t="inlineStr">
+      <c r="H14" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 30010008, 'retInfo': 验证码错误}</t>
         </is>
       </c>
-      <c r="I14" s="27" t="inlineStr">
+      <c r="I14" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
@@ -2408,7 +1839,7 @@
       <c r="J14" s="7" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" s="5" t="n">
+      <c r="A15" s="31" t="n">
         <v>14</v>
       </c>
       <c r="B15" s="6" t="n"/>
@@ -2437,12 +1868,12 @@
           <t>{"retCode": "19001", "retInfo": "渠道信息错误"}</t>
         </is>
       </c>
-      <c r="H15" s="26" t="inlineStr">
+      <c r="H15" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 19001, 'retInfo': 渠道信息错误}</t>
         </is>
       </c>
-      <c r="I15" s="27" t="inlineStr">
+      <c r="I15" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
@@ -2450,7 +1881,7 @@
       <c r="J15" s="7" t="n"/>
     </row>
     <row r="16">
-      <c r="A16" s="5" t="n">
+      <c r="A16" s="31" t="n">
         <v>15</v>
       </c>
       <c r="B16" s="6" t="n"/>
@@ -2479,12 +1910,12 @@
           <t>{"retCode": "19001", "retInfo": "手机号错误"}</t>
         </is>
       </c>
-      <c r="H16" s="31" t="inlineStr">
+      <c r="H16" s="40" t="inlineStr">
         <is>
           <t>{'retCode': 19001, 'retInfo': 手机号错误}</t>
         </is>
       </c>
-      <c r="I16" s="32" t="inlineStr">
+      <c r="I16" s="41" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
@@ -2492,7 +1923,7 @@
       <c r="J16" s="7" t="n"/>
     </row>
     <row r="17">
-      <c r="A17" s="5" t="n">
+      <c r="A17" s="31" t="n">
         <v>16</v>
       </c>
       <c r="B17" s="6" t="n"/>
@@ -2521,12 +1952,12 @@
           <t>{"retCode": "0", "retInfo": "ok","is_exist_db":"yes"}</t>
         </is>
       </c>
-      <c r="H17" s="26" t="inlineStr">
+      <c r="H17" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 0, 'retInfo': ok, 'is_exist_db': 'yes'}</t>
         </is>
       </c>
-      <c r="I17" s="27" t="inlineStr">
+      <c r="I17" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
@@ -2538,7 +1969,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="5" t="n">
+      <c r="A18" s="31" t="n">
         <v>17</v>
       </c>
       <c r="B18" s="7" t="inlineStr">
@@ -2571,12 +2002,12 @@
           <t>{"retCode": "20042023", "retInfo": "该手机号已被注册"}</t>
         </is>
       </c>
-      <c r="H18" s="31" t="inlineStr">
+      <c r="H18" s="40" t="inlineStr">
         <is>
           <t>{'retCode': 20042023, 'retInfo': 该手机号已被注册}</t>
         </is>
       </c>
-      <c r="I18" s="32" t="inlineStr">
+      <c r="I18" s="41" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
@@ -2597,81 +2028,81 @@
   </sheetPr>
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="1" width="6.375"/>
-    <col customWidth="1" max="2" min="2" style="1" width="11"/>
-    <col customWidth="1" max="3" min="3" style="1" width="28.625"/>
-    <col customWidth="1" max="4" min="4" style="1" width="52.625"/>
-    <col customWidth="1" max="5" min="5" style="1" width="66.625"/>
-    <col customWidth="1" max="6" min="6" style="1" width="12.75"/>
-    <col customWidth="1" max="7" min="7" style="1" width="11.625"/>
-    <col customWidth="1" max="8" min="8" style="1" width="6"/>
-    <col customWidth="1" max="9" min="9" style="1" width="5.875"/>
-    <col customWidth="1" max="10" min="10" style="1" width="90.75"/>
+    <col customWidth="1" max="1" min="1" style="36" width="6.375"/>
+    <col customWidth="1" max="2" min="2" style="36" width="11"/>
+    <col customWidth="1" max="3" min="3" style="36" width="28.625"/>
+    <col customWidth="1" max="4" min="4" style="36" width="52.625"/>
+    <col customWidth="1" max="5" min="5" style="36" width="66.625"/>
+    <col customWidth="1" max="6" min="6" style="36" width="12.75"/>
+    <col customWidth="1" max="7" min="7" style="36" width="11.625"/>
+    <col bestFit="1" customWidth="1" max="8" min="8" style="36" width="72.125"/>
+    <col customWidth="1" max="9" min="9" style="36" width="5.875"/>
+    <col customWidth="1" max="10" min="10" style="36" width="90.75"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="7" t="inlineStr">
+      <c r="A1" s="37" t="inlineStr">
         <is>
           <t>CaseId</t>
         </is>
       </c>
-      <c r="B1" s="7" t="inlineStr">
+      <c r="B1" s="37" t="inlineStr">
         <is>
           <t>Precondition</t>
         </is>
       </c>
-      <c r="C1" s="7" t="inlineStr">
+      <c r="C1" s="37" t="inlineStr">
         <is>
           <t>Title</t>
         </is>
       </c>
-      <c r="D1" s="7" t="inlineStr">
+      <c r="D1" s="37" t="inlineStr">
         <is>
           <t>URL</t>
         </is>
       </c>
-      <c r="E1" s="7" t="inlineStr">
+      <c r="E1" s="37" t="inlineStr">
         <is>
           <t>Data</t>
         </is>
       </c>
-      <c r="F1" s="7" t="inlineStr">
+      <c r="F1" s="37" t="inlineStr">
         <is>
           <t>ApiName</t>
         </is>
       </c>
-      <c r="G1" s="7" t="inlineStr">
+      <c r="G1" s="37" t="inlineStr">
         <is>
           <t>Expected</t>
         </is>
       </c>
-      <c r="H1" s="7" t="inlineStr">
+      <c r="H1" s="37" t="inlineStr">
         <is>
           <t>Actual</t>
         </is>
       </c>
-      <c r="I1" s="7" t="inlineStr">
+      <c r="I1" s="37" t="inlineStr">
         <is>
           <t>Result</t>
         </is>
       </c>
-      <c r="J1" s="7" t="inlineStr">
+      <c r="J1" s="37" t="inlineStr">
         <is>
           <t>Sql</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="n">
+      <c r="A2" s="31" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="inlineStr">
+      <c r="B2" s="31" t="inlineStr">
         <is>
           <t>无</t>
         </is>
@@ -2701,12 +2132,12 @@
           <t>{"retCode": "0", "retInfo": "ok"}</t>
         </is>
       </c>
-      <c r="H2" s="26" t="inlineStr">
+      <c r="H2" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 0, 'retInfo': ok}</t>
         </is>
       </c>
-      <c r="I2" s="27" t="inlineStr">
+      <c r="I2" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
@@ -2717,11 +2148,11 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="40.5" r="3" s="1">
-      <c r="A3" s="5" t="n">
+    <row customHeight="1" ht="40.5" r="3" s="36">
+      <c r="A3" s="31" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="12" t="n"/>
+      <c r="B3" s="33" t="n"/>
       <c r="C3" s="7" t="inlineStr">
         <is>
           <t>帐号注册</t>
@@ -2732,7 +2163,7 @@
           <t>/finance-user_info-war-1.0/ws/financeUserInfoFacade.ws?wsdl</t>
         </is>
       </c>
-      <c r="E3" s="25" t="inlineStr">
+      <c r="E3" s="23" t="inlineStr">
         <is>
           <t>{"verify_code": "${verify_code}", "user_id": "linux超${verify_unregistered_phone}", "channel_id": "1", "pwd": "123456", "mobile": "${verify_unregistered_phone}", "ip": "192.168.1.1"}</t>
         </is>
@@ -2747,12 +2178,12 @@
           <t>{"retCode": "0", "retInfo": "ok"}</t>
         </is>
       </c>
-      <c r="H3" s="26" t="inlineStr">
+      <c r="H3" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 0, 'retInfo': ok}</t>
         </is>
       </c>
-      <c r="I3" s="27" t="inlineStr">
+      <c r="I3" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
@@ -2764,10 +2195,10 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="n">
+      <c r="A4" s="31" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="inlineStr">
+      <c r="B4" s="31" t="inlineStr">
         <is>
           <t>用户已注册</t>
         </is>
@@ -2797,12 +2228,12 @@
           <t>{"retCode":"19001","retInfo":"用户ID错误"}</t>
         </is>
       </c>
-      <c r="H4" s="26" t="inlineStr">
+      <c r="H4" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 19001, 'retInfo': 用户ID错误}</t>
         </is>
       </c>
-      <c r="I4" s="27" t="inlineStr">
+      <c r="I4" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
@@ -2810,10 +2241,10 @@
       <c r="J4" s="7" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="n">
+      <c r="A5" s="31" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="11" t="n"/>
+      <c r="B5" s="32" t="n"/>
       <c r="C5" s="7" t="inlineStr">
         <is>
           <t>认证失败-真实姓名缺失</t>
@@ -2839,12 +2270,12 @@
           <t>{"retCode":"19001","retInfo": "真实姓名错误"}</t>
         </is>
       </c>
-      <c r="H5" s="26" t="inlineStr">
+      <c r="H5" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 19001, 'retInfo': 真实姓名错误}</t>
         </is>
       </c>
-      <c r="I5" s="27" t="inlineStr">
+      <c r="I5" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
@@ -2852,10 +2283,10 @@
       <c r="J5" s="7" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="5" t="n">
+      <c r="A6" s="31" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="11" t="n"/>
+      <c r="B6" s="32" t="n"/>
       <c r="C6" s="7" t="inlineStr">
         <is>
           <t>认证失败-身份证号缺失</t>
@@ -2881,12 +2312,12 @@
           <t>{"retCode":"19001","retInfo": "身份证号错误"}</t>
         </is>
       </c>
-      <c r="H6" s="26" t="inlineStr">
+      <c r="H6" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 19001, 'retInfo': 身份证号错误}</t>
         </is>
       </c>
-      <c r="I6" s="27" t="inlineStr">
+      <c r="I6" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
@@ -2894,10 +2325,10 @@
       <c r="J6" s="7" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" s="5" t="n">
+      <c r="A7" s="31" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="11" t="n"/>
+      <c r="B7" s="32" t="n"/>
       <c r="C7" s="7" t="inlineStr">
         <is>
           <t>认证失败-uid为空</t>
@@ -2923,12 +2354,12 @@
           <t>{"retCode":"19001","retInfo": "用户ID错误"}</t>
         </is>
       </c>
-      <c r="H7" s="26" t="inlineStr">
+      <c r="H7" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 19001, 'retInfo': 用户ID错误}</t>
         </is>
       </c>
-      <c r="I7" s="27" t="inlineStr">
+      <c r="I7" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
@@ -2936,10 +2367,10 @@
       <c r="J7" s="7" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="5" t="n">
+      <c r="A8" s="31" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="11" t="n"/>
+      <c r="B8" s="32" t="n"/>
       <c r="C8" s="7" t="inlineStr">
         <is>
           <t>认证失败-真实姓名为空</t>
@@ -2965,12 +2396,12 @@
           <t>{"retCode":"19001","retInfo": "真实姓名错误"}</t>
         </is>
       </c>
-      <c r="H8" s="26" t="inlineStr">
+      <c r="H8" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 19001, 'retInfo': 真实姓名错误}</t>
         </is>
       </c>
-      <c r="I8" s="27" t="inlineStr">
+      <c r="I8" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
@@ -2978,10 +2409,10 @@
       <c r="J8" s="7" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="5" t="n">
+      <c r="A9" s="31" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="11" t="n"/>
+      <c r="B9" s="32" t="n"/>
       <c r="C9" s="7" t="inlineStr">
         <is>
           <t>认证失败-身份证号为空</t>
@@ -3007,12 +2438,12 @@
           <t>{"retCode":"19001","retInfo": "身份证号错误"}</t>
         </is>
       </c>
-      <c r="H9" s="26" t="inlineStr">
+      <c r="H9" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 19001, 'retInfo': 身份证号错误}</t>
         </is>
       </c>
-      <c r="I9" s="27" t="inlineStr">
+      <c r="I9" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
@@ -3020,10 +2451,10 @@
       <c r="J9" s="7" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" s="5" t="n">
+      <c r="A10" s="31" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="11" t="n"/>
+      <c r="B10" s="32" t="n"/>
       <c r="C10" s="7" t="inlineStr">
         <is>
           <t>认证失败-uid错误</t>
@@ -3049,12 +2480,12 @@
           <t>{"retCode":"20042002","retInfo": "用户不存在"}</t>
         </is>
       </c>
-      <c r="H10" s="26" t="inlineStr">
+      <c r="H10" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 20042002, 'retInfo': 用户不存在}</t>
         </is>
       </c>
-      <c r="I10" s="27" t="inlineStr">
+      <c r="I10" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
@@ -3062,10 +2493,10 @@
       <c r="J10" s="7" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="5" t="n">
+      <c r="A11" s="31" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="11" t="n"/>
+      <c r="B11" s="32" t="n"/>
       <c r="C11" s="7" t="inlineStr">
         <is>
           <t>认证失败-真实姓名为非中文</t>
@@ -3091,12 +2522,12 @@
           <t>{"retCode":"19001","retInfo": "真实姓名必须为中文"}</t>
         </is>
       </c>
-      <c r="H11" s="26" t="inlineStr">
+      <c r="H11" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 19001, 'retInfo': 真实姓名必须为中文}</t>
         </is>
       </c>
-      <c r="I11" s="27" t="inlineStr">
+      <c r="I11" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
@@ -3104,10 +2535,10 @@
       <c r="J11" s="7" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" s="5" t="n">
+      <c r="A12" s="31" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="11" t="n"/>
+      <c r="B12" s="32" t="n"/>
       <c r="C12" s="7" t="inlineStr">
         <is>
           <t>认证失败-真实姓名错误</t>
@@ -3133,12 +2564,12 @@
           <t>{"retCode":"0","retInfo": "ok","Flstate":"无效"}</t>
         </is>
       </c>
-      <c r="H12" s="26" t="inlineStr">
+      <c r="H12" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 0, 'retInfo': ok, 'Flstate': '有效'}</t>
         </is>
       </c>
-      <c r="I12" s="28" t="inlineStr">
+      <c r="I12" s="42" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
@@ -3150,10 +2581,10 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="5" t="n">
+      <c r="A13" s="31" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="11" t="n"/>
+      <c r="B13" s="32" t="n"/>
       <c r="C13" s="7" t="inlineStr">
         <is>
           <t>认证失败-身份证号错误</t>
@@ -3179,12 +2610,12 @@
           <t>{"retCode":"19001","retInfo": "身份证号检验错误"}</t>
         </is>
       </c>
-      <c r="H13" s="26" t="inlineStr">
+      <c r="H13" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 19001, 'retInfo': 身份证号检验错误}</t>
         </is>
       </c>
-      <c r="I13" s="27" t="inlineStr">
+      <c r="I13" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
@@ -3192,10 +2623,10 @@
       <c r="J13" s="7" t="n"/>
     </row>
     <row r="14">
-      <c r="A14" s="5" t="n">
+      <c r="A14" s="31" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="11" t="n"/>
+      <c r="B14" s="32" t="n"/>
       <c r="C14" s="7" t="inlineStr">
         <is>
           <t>认证失败-身份证号小于18位</t>
@@ -3221,12 +2652,12 @@
           <t>{"retCode":"100010000","retInfo": "不是18位的身份证号码"}</t>
         </is>
       </c>
-      <c r="H14" s="26" t="inlineStr">
+      <c r="H14" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 100010000, 'retInfo': 不是18位的身份证号码}</t>
         </is>
       </c>
-      <c r="I14" s="27" t="inlineStr">
+      <c r="I14" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
@@ -3234,10 +2665,10 @@
       <c r="J14" s="7" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" s="5" t="n">
+      <c r="A15" s="31" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="11" t="n"/>
+      <c r="B15" s="32" t="n"/>
       <c r="C15" s="7" t="inlineStr">
         <is>
           <t>认证失败-身份证号大于18位</t>
@@ -3263,12 +2694,12 @@
           <t>{"retCode":"19001","retInfo": "身份证号错误"}</t>
         </is>
       </c>
-      <c r="H15" s="26" t="inlineStr">
+      <c r="H15" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 19001, 'retInfo': 身份证号错误}</t>
         </is>
       </c>
-      <c r="I15" s="27" t="inlineStr">
+      <c r="I15" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
@@ -3276,10 +2707,10 @@
       <c r="J15" s="7" t="n"/>
     </row>
     <row r="16">
-      <c r="A16" s="5" t="n">
+      <c r="A16" s="31" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="11" t="n"/>
+      <c r="B16" s="32" t="n"/>
       <c r="C16" s="7" t="inlineStr">
         <is>
           <t>认证成功-真实姓名正确</t>
@@ -3305,12 +2736,12 @@
           <t>{"retCode":"0","retInfo": "ok","Flstate":"有效"}</t>
         </is>
       </c>
-      <c r="H16" s="31" t="inlineStr">
+      <c r="H16" s="40" t="inlineStr">
         <is>
           <t>{'retCode': 0, 'retInfo': ok, 'Flstate': '有效'}</t>
         </is>
       </c>
-      <c r="I16" s="27" t="inlineStr">
+      <c r="I16" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
@@ -3322,10 +2753,10 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="5" t="n">
+      <c r="A17" s="31" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="12" t="n"/>
+      <c r="B17" s="33" t="n"/>
       <c r="C17" s="7" t="inlineStr">
         <is>
           <t>认证失败-身份证已经被认证</t>
@@ -3351,12 +2782,12 @@
           <t>{"retCode":"20042033","retInfo": "该身份证已经进行过实名认证"}</t>
         </is>
       </c>
-      <c r="H17" s="31" t="inlineStr">
+      <c r="H17" s="40" t="inlineStr">
         <is>
           <t>{'retCode': 20042033, 'retInfo': 该身份证已经进行过实名认证}</t>
         </is>
       </c>
-      <c r="I17" s="27" t="inlineStr">
+      <c r="I17" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
@@ -3364,10 +2795,10 @@
       <c r="J17" s="15" t="n"/>
     </row>
     <row r="18">
-      <c r="A18" s="5" t="n">
+      <c r="A18" s="31" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="5" t="inlineStr">
+      <c r="B18" s="31" t="inlineStr">
         <is>
           <t>用户未注册</t>
         </is>
@@ -3397,12 +2828,12 @@
           <t>{"retCode":"20042002","retInfo": "用户不存在"}</t>
         </is>
       </c>
-      <c r="H18" s="26" t="inlineStr">
+      <c r="H18" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 20042002, 'retInfo': 用户不存在}</t>
         </is>
       </c>
-      <c r="I18" s="27" t="inlineStr">
+      <c r="I18" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
@@ -3426,81 +2857,81 @@
   </sheetPr>
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F4" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="1" width="6.375"/>
-    <col customWidth="1" max="2" min="2" style="1" width="23.875"/>
+    <col customWidth="1" max="1" min="1" style="36" width="6.375"/>
+    <col customWidth="1" max="2" min="2" style="36" width="23.875"/>
     <col customWidth="1" max="3" min="3" style="20" width="43.875"/>
     <col customWidth="1" max="4" min="4" style="20" width="4.375"/>
     <col customWidth="1" max="5" min="5" style="20" width="167.625"/>
-    <col customWidth="1" max="6" min="6" style="1" width="12.375"/>
+    <col customWidth="1" max="6" min="6" style="36" width="12.375"/>
     <col customWidth="1" max="7" min="7" style="20" width="46.625"/>
-    <col customWidth="1" max="8" min="8" style="1" width="71.875"/>
-    <col customWidth="1" max="9" min="9" style="1" width="5.875"/>
-    <col customWidth="1" max="10" min="10" style="1" width="90.75"/>
+    <col customWidth="1" max="8" min="8" style="36" width="71.875"/>
+    <col customWidth="1" max="9" min="9" style="36" width="5.875"/>
+    <col customWidth="1" max="10" min="10" style="36" width="90.75"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="7" t="inlineStr">
+      <c r="A1" s="37" t="inlineStr">
         <is>
           <t>CaseId</t>
         </is>
       </c>
-      <c r="B1" s="7" t="inlineStr">
+      <c r="B1" s="37" t="inlineStr">
         <is>
           <t>Precondition</t>
         </is>
       </c>
-      <c r="C1" s="7" t="inlineStr">
+      <c r="C1" s="37" t="inlineStr">
         <is>
           <t>Title</t>
         </is>
       </c>
-      <c r="D1" s="7" t="inlineStr">
+      <c r="D1" s="37" t="inlineStr">
         <is>
           <t>URL</t>
         </is>
       </c>
-      <c r="E1" s="7" t="inlineStr">
+      <c r="E1" s="37" t="inlineStr">
         <is>
           <t>Data</t>
         </is>
       </c>
-      <c r="F1" s="7" t="inlineStr">
+      <c r="F1" s="37" t="inlineStr">
         <is>
           <t>ApiName</t>
         </is>
       </c>
-      <c r="G1" s="7" t="inlineStr">
+      <c r="G1" s="37" t="inlineStr">
         <is>
           <t>Expected</t>
         </is>
       </c>
-      <c r="H1" s="7" t="inlineStr">
+      <c r="H1" s="37" t="inlineStr">
         <is>
           <t>Actual</t>
         </is>
       </c>
-      <c r="I1" s="7" t="inlineStr">
+      <c r="I1" s="37" t="inlineStr">
         <is>
           <t>Result</t>
         </is>
       </c>
-      <c r="J1" s="7" t="inlineStr">
+      <c r="J1" s="37" t="inlineStr">
         <is>
           <t>Sql</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="n">
+      <c r="A2" s="31" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="21" t="inlineStr">
+      <c r="B2" s="34" t="inlineStr">
         <is>
           <t>无</t>
         </is>
@@ -3530,12 +2961,12 @@
           <t>{"retCode": "0", "retInfo": "ok"}</t>
         </is>
       </c>
-      <c r="H2" s="26" t="inlineStr">
+      <c r="H2" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 0, 'retInfo': ok}</t>
         </is>
       </c>
-      <c r="I2" s="27" t="inlineStr">
+      <c r="I2" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
@@ -3547,10 +2978,10 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="n">
+      <c r="A3" s="31" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="11" t="n"/>
+      <c r="B3" s="32" t="n"/>
       <c r="C3" s="7" t="inlineStr">
         <is>
           <t>帐号注册</t>
@@ -3576,12 +3007,12 @@
           <t>{"retCode": "0", "retInfo": "ok"}</t>
         </is>
       </c>
-      <c r="H3" s="26" t="inlineStr">
+      <c r="H3" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 0, 'retInfo': ok}</t>
         </is>
       </c>
-      <c r="I3" s="27" t="inlineStr">
+      <c r="I3" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
@@ -3593,10 +3024,10 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="n">
+      <c r="A4" s="31" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="11" t="n"/>
+      <c r="B4" s="32" t="n"/>
       <c r="C4" s="7" t="inlineStr">
         <is>
           <t>实名认证</t>
@@ -3622,28 +3053,28 @@
           <t>{"retCode":"0","retInfo": "ok"}</t>
         </is>
       </c>
-      <c r="H4" s="26" t="inlineStr">
+      <c r="H4" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 0, 'retInfo': ok}</t>
         </is>
       </c>
-      <c r="I4" s="27" t="inlineStr">
+      <c r="I4" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
       </c>
       <c r="J4" s="7" t="n"/>
     </row>
-    <row customHeight="1" ht="14.25" r="5" s="1">
-      <c r="A5" s="22" t="n">
+    <row customHeight="1" ht="14.25" r="5" s="36">
+      <c r="A5" s="21" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="23" t="inlineStr">
+      <c r="B5" s="35" t="inlineStr">
         <is>
           <t>账户已实名认证</t>
         </is>
       </c>
-      <c r="C5" s="24" t="inlineStr">
+      <c r="C5" s="22" t="inlineStr">
         <is>
           <t>绑定失败-uid缺失</t>
         </is>
@@ -3668,23 +3099,23 @@
           <t>{"retCode":"19001","retInfo":"用户UID错误"}</t>
         </is>
       </c>
-      <c r="H5" s="26" t="inlineStr">
+      <c r="H5" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 19001, 'retInfo': 用户UID错误}</t>
         </is>
       </c>
-      <c r="I5" s="27" t="inlineStr">
+      <c r="I5" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
       </c>
       <c r="J5" s="7" t="n"/>
     </row>
-    <row customHeight="1" ht="14.25" r="6" s="1">
-      <c r="A6" s="22" t="n">
+    <row customHeight="1" ht="14.25" r="6" s="36">
+      <c r="A6" s="21" t="n">
         <v>5</v>
       </c>
-      <c r="C6" s="24" t="inlineStr">
+      <c r="C6" s="22" t="inlineStr">
         <is>
           <t>绑定失败-支付密码缺失</t>
         </is>
@@ -3709,23 +3140,23 @@
           <t>{"retCode":"19001","retInfo":"支付密码错误"}</t>
         </is>
       </c>
-      <c r="H6" s="26" t="inlineStr">
+      <c r="H6" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 19001, 'retInfo': 支付密码错误}</t>
         </is>
       </c>
-      <c r="I6" s="27" t="inlineStr">
+      <c r="I6" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
       </c>
       <c r="J6" s="7" t="n"/>
     </row>
-    <row customHeight="1" ht="14.25" r="7" s="1">
-      <c r="A7" s="22" t="n">
+    <row customHeight="1" ht="14.25" r="7" s="36">
+      <c r="A7" s="21" t="n">
         <v>6</v>
       </c>
-      <c r="C7" s="24" t="inlineStr">
+      <c r="C7" s="22" t="inlineStr">
         <is>
           <t>绑定失败-绑定的银行卡手机号缺失</t>
         </is>
@@ -3750,23 +3181,23 @@
           <t>{"retCode":"19001","retInfo":"绑定的银行卡手机号错误"}</t>
         </is>
       </c>
-      <c r="H7" s="26" t="inlineStr">
+      <c r="H7" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 19001, 'retInfo': 绑定的银行卡手机号错误}</t>
         </is>
       </c>
-      <c r="I7" s="27" t="inlineStr">
+      <c r="I7" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
       </c>
       <c r="J7" s="7" t="n"/>
     </row>
-    <row customHeight="1" ht="14.25" r="8" s="1">
-      <c r="A8" s="22" t="n">
+    <row customHeight="1" ht="14.25" r="8" s="36">
+      <c r="A8" s="21" t="n">
         <v>7</v>
       </c>
-      <c r="C8" s="24" t="inlineStr">
+      <c r="C8" s="22" t="inlineStr">
         <is>
           <t>绑定失败-证件ID缺失</t>
         </is>
@@ -3791,23 +3222,23 @@
           <t>{"retCode":"19001","retInfo":"证件号错误"}</t>
         </is>
       </c>
-      <c r="H8" s="26" t="inlineStr">
+      <c r="H8" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 19001, 'retInfo': 证件号错误}</t>
         </is>
       </c>
-      <c r="I8" s="27" t="inlineStr">
+      <c r="I8" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
       </c>
       <c r="J8" s="7" t="n"/>
     </row>
-    <row customHeight="1" ht="14.25" r="9" s="1">
-      <c r="A9" s="22" t="n">
+    <row customHeight="1" ht="14.25" r="9" s="36">
+      <c r="A9" s="21" t="n">
         <v>8</v>
       </c>
-      <c r="C9" s="24" t="inlineStr">
+      <c r="C9" s="22" t="inlineStr">
         <is>
           <t>绑定失败-持卡人姓名缺失</t>
         </is>
@@ -3832,23 +3263,23 @@
           <t>{"retCode":"19001","retInfo":"持卡人姓名错误"}</t>
         </is>
       </c>
-      <c r="H9" s="26" t="inlineStr">
+      <c r="H9" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 19001, 'retInfo': 持卡人姓名错误}</t>
         </is>
       </c>
-      <c r="I9" s="27" t="inlineStr">
+      <c r="I9" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
       </c>
       <c r="J9" s="7" t="n"/>
     </row>
-    <row customHeight="1" ht="14.25" r="10" s="1">
-      <c r="A10" s="22" t="n">
+    <row customHeight="1" ht="14.25" r="10" s="36">
+      <c r="A10" s="21" t="n">
         <v>9</v>
       </c>
-      <c r="C10" s="24" t="inlineStr">
+      <c r="C10" s="22" t="inlineStr">
         <is>
           <t>绑定失败-卡号缺失</t>
         </is>
@@ -3873,23 +3304,23 @@
           <t>{"retCode":"19001","retInfo":"卡号错误"}</t>
         </is>
       </c>
-      <c r="H10" s="26" t="inlineStr">
+      <c r="H10" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 19001, 'retInfo': 卡号错误}</t>
         </is>
       </c>
-      <c r="I10" s="27" t="inlineStr">
+      <c r="I10" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
       </c>
       <c r="J10" s="7" t="n"/>
     </row>
-    <row customHeight="1" ht="14.25" r="11" s="1">
-      <c r="A11" s="22" t="n">
+    <row customHeight="1" ht="14.25" r="11" s="36">
+      <c r="A11" s="21" t="n">
         <v>10</v>
       </c>
-      <c r="C11" s="24" t="inlineStr">
+      <c r="C11" s="22" t="inlineStr">
         <is>
           <t>绑定失败-银行卡类型缺失</t>
         </is>
@@ -3914,23 +3345,23 @@
           <t>{"retCode":"19001","retInfo":"银行类型错误"}</t>
         </is>
       </c>
-      <c r="H11" s="26" t="inlineStr">
+      <c r="H11" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 19001, 'retInfo': 银行类型错误}</t>
         </is>
       </c>
-      <c r="I11" s="27" t="inlineStr">
+      <c r="I11" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
       </c>
       <c r="J11" s="7" t="n"/>
     </row>
-    <row customHeight="1" ht="14.25" r="12" s="1">
-      <c r="A12" s="22" t="n">
+    <row customHeight="1" ht="14.25" r="12" s="36">
+      <c r="A12" s="21" t="n">
         <v>11</v>
       </c>
-      <c r="C12" s="24" t="inlineStr">
+      <c r="C12" s="22" t="inlineStr">
         <is>
           <t>绑定失败-银行名称缺失</t>
         </is>
@@ -3955,23 +3386,23 @@
           <t>{"retCode":"19001","retInfo":"银行卡号检验错误"}</t>
         </is>
       </c>
-      <c r="H12" s="26" t="inlineStr">
+      <c r="H12" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 20042018, 'retInfo': 用户交易密码不正确或未配置}</t>
         </is>
       </c>
-      <c r="I12" s="28" t="inlineStr">
+      <c r="I12" s="42" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
       <c r="J12" s="7" t="n"/>
     </row>
-    <row customHeight="1" ht="14.25" r="13" s="1">
-      <c r="A13" s="22" t="n">
+    <row customHeight="1" ht="14.25" r="13" s="36">
+      <c r="A13" s="21" t="n">
         <v>12</v>
       </c>
-      <c r="C13" s="24" t="inlineStr">
+      <c r="C13" s="22" t="inlineStr">
         <is>
           <t>绑定失败-uid为空</t>
         </is>
@@ -3996,23 +3427,23 @@
           <t>{"retCode":"19001","retInfo":"用户UID错误"}</t>
         </is>
       </c>
-      <c r="H13" s="26" t="inlineStr">
+      <c r="H13" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 19001, 'retInfo': 用户UID错误}</t>
         </is>
       </c>
-      <c r="I13" s="27" t="inlineStr">
+      <c r="I13" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
       </c>
       <c r="J13" s="7" t="n"/>
     </row>
-    <row customHeight="1" ht="14.25" r="14" s="1">
-      <c r="A14" s="22" t="n">
+    <row customHeight="1" ht="14.25" r="14" s="36">
+      <c r="A14" s="21" t="n">
         <v>13</v>
       </c>
-      <c r="C14" s="24" t="inlineStr">
+      <c r="C14" s="22" t="inlineStr">
         <is>
           <t>绑定失败-支付密码为空</t>
         </is>
@@ -4037,23 +3468,23 @@
           <t>{"retCode":"19001","retInfo":"支付密码错误"}</t>
         </is>
       </c>
-      <c r="H14" s="26" t="inlineStr">
+      <c r="H14" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 19001, 'retInfo': 支付密码错误}</t>
         </is>
       </c>
-      <c r="I14" s="27" t="inlineStr">
+      <c r="I14" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
       </c>
       <c r="J14" s="7" t="n"/>
     </row>
-    <row customHeight="1" ht="14.25" r="15" s="1">
-      <c r="A15" s="22" t="n">
+    <row customHeight="1" ht="14.25" r="15" s="36">
+      <c r="A15" s="21" t="n">
         <v>14</v>
       </c>
-      <c r="C15" s="24" t="inlineStr">
+      <c r="C15" s="22" t="inlineStr">
         <is>
           <t>绑定失败-绑定的银行卡手机号为空</t>
         </is>
@@ -4078,23 +3509,23 @@
           <t>{"retCode":"19001","retInfo":"绑定的银行卡手机号错误"}</t>
         </is>
       </c>
-      <c r="H15" s="26" t="inlineStr">
+      <c r="H15" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 19001, 'retInfo': 绑定的银行卡手机号错误}</t>
         </is>
       </c>
-      <c r="I15" s="27" t="inlineStr">
+      <c r="I15" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
       </c>
       <c r="J15" s="7" t="n"/>
     </row>
-    <row customHeight="1" ht="14.25" r="16" s="1">
-      <c r="A16" s="22" t="n">
+    <row customHeight="1" ht="14.25" r="16" s="36">
+      <c r="A16" s="21" t="n">
         <v>15</v>
       </c>
-      <c r="C16" s="24" t="inlineStr">
+      <c r="C16" s="22" t="inlineStr">
         <is>
           <t>绑定失败-证件ID为空</t>
         </is>
@@ -4119,23 +3550,23 @@
           <t>{"retCode":"19001","retInfo":"证件号错误"}</t>
         </is>
       </c>
-      <c r="H16" s="26" t="inlineStr">
+      <c r="H16" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 19001, 'retInfo': 证件号错误}</t>
         </is>
       </c>
-      <c r="I16" s="27" t="inlineStr">
+      <c r="I16" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
       </c>
       <c r="J16" s="7" t="n"/>
     </row>
-    <row customHeight="1" ht="14.25" r="17" s="1">
-      <c r="A17" s="22" t="n">
+    <row customHeight="1" ht="14.25" r="17" s="36">
+      <c r="A17" s="21" t="n">
         <v>16</v>
       </c>
-      <c r="C17" s="24" t="inlineStr">
+      <c r="C17" s="22" t="inlineStr">
         <is>
           <t>绑定失败-持卡人姓名为空</t>
         </is>
@@ -4160,23 +3591,23 @@
           <t>{"retCode":"19001","retInfo":"持卡人姓名错误"}</t>
         </is>
       </c>
-      <c r="H17" s="26" t="inlineStr">
+      <c r="H17" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 19001, 'retInfo': 持卡人姓名错误}</t>
         </is>
       </c>
-      <c r="I17" s="27" t="inlineStr">
+      <c r="I17" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
       </c>
       <c r="J17" s="7" t="n"/>
     </row>
-    <row customHeight="1" ht="14.25" r="18" s="1">
-      <c r="A18" s="22" t="n">
+    <row customHeight="1" ht="14.25" r="18" s="36">
+      <c r="A18" s="21" t="n">
         <v>17</v>
       </c>
-      <c r="C18" s="24" t="inlineStr">
+      <c r="C18" s="22" t="inlineStr">
         <is>
           <t>绑定失败-卡号为空</t>
         </is>
@@ -4201,23 +3632,23 @@
           <t>{"retCode":"19001","retInfo":"卡号错误"}</t>
         </is>
       </c>
-      <c r="H18" s="26" t="inlineStr">
+      <c r="H18" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 19001, 'retInfo': 卡号错误}</t>
         </is>
       </c>
-      <c r="I18" s="27" t="inlineStr">
+      <c r="I18" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
       </c>
       <c r="J18" s="7" t="n"/>
     </row>
-    <row customHeight="1" ht="14.25" r="19" s="1">
-      <c r="A19" s="22" t="n">
+    <row customHeight="1" ht="14.25" r="19" s="36">
+      <c r="A19" s="21" t="n">
         <v>18</v>
       </c>
-      <c r="C19" s="24" t="inlineStr">
+      <c r="C19" s="22" t="inlineStr">
         <is>
           <t>绑定失败-银行卡类型为空</t>
         </is>
@@ -4242,23 +3673,23 @@
           <t>{"retCode":"19001","retInfo":"银行类型错误"}</t>
         </is>
       </c>
-      <c r="H19" s="26" t="inlineStr">
+      <c r="H19" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 19001, 'retInfo': 银行类型错误}</t>
         </is>
       </c>
-      <c r="I19" s="27" t="inlineStr">
+      <c r="I19" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
       </c>
       <c r="J19" s="7" t="n"/>
     </row>
-    <row customHeight="1" ht="14.25" r="20" s="1">
-      <c r="A20" s="22" t="n">
+    <row customHeight="1" ht="14.25" r="20" s="36">
+      <c r="A20" s="21" t="n">
         <v>19</v>
       </c>
-      <c r="C20" s="24" t="inlineStr">
+      <c r="C20" s="22" t="inlineStr">
         <is>
           <t>绑定失败-银行名称为空</t>
         </is>
@@ -4283,23 +3714,23 @@
           <t>{"retCode":"19001","retInfo":"银行卡号检验错误"}</t>
         </is>
       </c>
-      <c r="H20" s="26" t="inlineStr">
+      <c r="H20" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 20042018, 'retInfo': 用户交易密码不正确或未配置}</t>
         </is>
       </c>
-      <c r="I20" s="28" t="inlineStr">
+      <c r="I20" s="42" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
       <c r="J20" s="7" t="n"/>
     </row>
-    <row customHeight="1" ht="14.25" r="21" s="1">
-      <c r="A21" s="22" t="n">
+    <row customHeight="1" ht="14.25" r="21" s="36">
+      <c r="A21" s="21" t="n">
         <v>20</v>
       </c>
-      <c r="C21" s="24" t="inlineStr">
+      <c r="C21" s="22" t="inlineStr">
         <is>
           <t>绑定失败-银行卡号18位错误</t>
         </is>
@@ -4324,23 +3755,23 @@
           <t>{"retCode":"19001","retInfo":"银行卡号检验错误"}</t>
         </is>
       </c>
-      <c r="H21" s="26" t="inlineStr">
+      <c r="H21" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 19001, 'retInfo': 银行卡号检验错误}</t>
         </is>
       </c>
-      <c r="I21" s="27" t="inlineStr">
+      <c r="I21" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
       </c>
       <c r="J21" s="7" t="n"/>
     </row>
-    <row customHeight="1" ht="14.25" r="22" s="1">
-      <c r="A22" s="22" t="n">
+    <row customHeight="1" ht="14.25" r="22" s="36">
+      <c r="A22" s="21" t="n">
         <v>21</v>
       </c>
-      <c r="C22" s="24" t="inlineStr">
+      <c r="C22" s="22" t="inlineStr">
         <is>
           <t>绑定失败-银行名称错误</t>
         </is>
@@ -4365,23 +3796,23 @@
           <t>{"retCode":"20042006","retInfo":"用户实名信息比对错误"}</t>
         </is>
       </c>
-      <c r="H22" s="26" t="inlineStr">
+      <c r="H22" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 20042018, 'retInfo': 用户交易密码不正确或未配置}</t>
         </is>
       </c>
-      <c r="I22" s="28" t="inlineStr">
+      <c r="I22" s="42" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
       <c r="J22" s="7" t="n"/>
     </row>
-    <row customHeight="1" ht="14.25" r="23" s="1">
-      <c r="A23" s="22" t="n">
+    <row customHeight="1" ht="14.25" r="23" s="36">
+      <c r="A23" s="21" t="n">
         <v>22</v>
       </c>
-      <c r="C23" s="24" t="inlineStr">
+      <c r="C23" s="22" t="inlineStr">
         <is>
           <t>绑定失败-证件ID与实名时身份证号不一致</t>
         </is>
@@ -4406,23 +3837,23 @@
           <t>{"retCode":"20042006","retInfo":"用户实名信息比对错误"}</t>
         </is>
       </c>
-      <c r="H23" s="26" t="inlineStr">
+      <c r="H23" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 20042006, 'retInfo': 用户实名信息比对错误}</t>
         </is>
       </c>
-      <c r="I23" s="27" t="inlineStr">
+      <c r="I23" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
       </c>
       <c r="J23" s="7" t="n"/>
     </row>
-    <row customHeight="1" ht="14.25" r="24" s="1">
-      <c r="A24" s="22" t="n">
+    <row customHeight="1" ht="14.25" r="24" s="36">
+      <c r="A24" s="21" t="n">
         <v>23</v>
       </c>
-      <c r="C24" s="24" t="inlineStr">
+      <c r="C24" s="22" t="inlineStr">
         <is>
           <t>绑定失败-银行卡手机号非11位</t>
         </is>
@@ -4447,23 +3878,23 @@
           <t>{"retCode":"19001","retInfo":"绑定的银行卡手机号错误"}</t>
         </is>
       </c>
-      <c r="H24" s="26" t="inlineStr">
+      <c r="H24" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 19001, 'retInfo': 绑定的银行卡手机号错误}</t>
         </is>
       </c>
-      <c r="I24" s="27" t="inlineStr">
+      <c r="I24" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
       </c>
       <c r="J24" s="7" t="n"/>
     </row>
-    <row customHeight="1" ht="14.25" r="25" s="1">
-      <c r="A25" s="22" t="n">
+    <row customHeight="1" ht="14.25" r="25" s="36">
+      <c r="A25" s="21" t="n">
         <v>24</v>
       </c>
-      <c r="C25" s="24" t="inlineStr">
+      <c r="C25" s="22" t="inlineStr">
         <is>
           <t>绑定失败-持卡人姓名错误</t>
         </is>
@@ -4488,23 +3919,23 @@
           <t>{"retCode":"20042006","retInfo":"用户实名信息比对错误"}</t>
         </is>
       </c>
-      <c r="H25" s="26" t="inlineStr">
+      <c r="H25" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 20042006, 'retInfo': 用户实名信息比对错误}</t>
         </is>
       </c>
-      <c r="I25" s="27" t="inlineStr">
+      <c r="I25" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
       </c>
       <c r="J25" s="7" t="n"/>
     </row>
-    <row customHeight="1" ht="14.25" r="26" s="1">
-      <c r="A26" s="22" t="n">
+    <row customHeight="1" ht="14.25" r="26" s="36">
+      <c r="A26" s="21" t="n">
         <v>25</v>
       </c>
-      <c r="C26" s="24" t="inlineStr">
+      <c r="C26" s="22" t="inlineStr">
         <is>
           <t>绑定失败-银行卡号格式错误(大于18位)</t>
         </is>
@@ -4529,23 +3960,23 @@
           <t>{"retCode":"19001","retInfo":"卡号错误"}</t>
         </is>
       </c>
-      <c r="H26" s="26" t="inlineStr">
+      <c r="H26" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 19001, 'retInfo': 卡号错误}</t>
         </is>
       </c>
-      <c r="I26" s="27" t="inlineStr">
+      <c r="I26" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
       </c>
       <c r="J26" s="7" t="n"/>
     </row>
-    <row customHeight="1" ht="14.25" r="27" s="1">
-      <c r="A27" s="22" t="n">
+    <row customHeight="1" ht="14.25" r="27" s="36">
+      <c r="A27" s="21" t="n">
         <v>26</v>
       </c>
-      <c r="C27" s="24" t="inlineStr">
+      <c r="C27" s="22" t="inlineStr">
         <is>
           <t>绑定失败-银行类型错误</t>
         </is>
@@ -4570,23 +4001,23 @@
           <t>{"retCode":"20042006","retInfo":"用户实名信息比对错误"}</t>
         </is>
       </c>
-      <c r="H27" s="26" t="inlineStr">
+      <c r="H27" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 20042018, 'retInfo': 用户交易密码不正确或未配置}</t>
         </is>
       </c>
-      <c r="I27" s="28" t="inlineStr">
+      <c r="I27" s="42" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
       <c r="J27" s="7" t="n"/>
     </row>
-    <row customHeight="1" ht="14.25" r="28" s="1">
-      <c r="A28" s="22" t="n">
+    <row customHeight="1" ht="14.25" r="28" s="36">
+      <c r="A28" s="21" t="n">
         <v>27</v>
       </c>
-      <c r="C28" s="24" t="inlineStr">
+      <c r="C28" s="22" t="inlineStr">
         <is>
           <t>绑定成功-所有参数正确</t>
         </is>
@@ -4611,22 +4042,22 @@
           <t>{"retCode": "0", "retInfo": "ok"}</t>
         </is>
       </c>
-      <c r="H28" s="29" t="inlineStr">
+      <c r="H28" s="43" t="inlineStr">
         <is>
           <t>{'retCode': 20042018, 'retInfo': 用户交易密码不正确或未配置}</t>
         </is>
       </c>
-      <c r="I28" s="30" t="inlineStr">
+      <c r="I28" s="44" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="14.25" r="29" s="1">
-      <c r="A29" s="5" t="n">
+    <row customHeight="1" ht="14.25" r="29" s="36">
+      <c r="A29" s="31" t="n">
         <v>28</v>
       </c>
-      <c r="B29" s="5" t="inlineStr">
+      <c r="B29" s="31" t="inlineStr">
         <is>
           <t>账户未实名认证</t>
         </is>
@@ -4656,12 +4087,12 @@
           <t>{"retCode":"20042004","retInfo":"用户实名认证信息不存在"}</t>
         </is>
       </c>
-      <c r="H29" s="26" t="inlineStr">
+      <c r="H29" s="38" t="inlineStr">
         <is>
           <t>{'retCode': 20042004, 'retInfo': 用户实名认证信息不存在}</t>
         </is>
       </c>
-      <c r="I29" s="27" t="inlineStr">
+      <c r="I29" s="39" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
@@ -4687,12 +4118,12 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A28" sqref="$A28:$XFD28"/>
+      <selection activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" max="3" min="3" style="1" width="24.875"/>
+    <col customWidth="1" max="3" min="3" style="36" width="24.875"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4733,7 +4164,7 @@
       <c r="I1" s="15" t="n"/>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="n">
+      <c r="A2" s="31" t="n">
         <v>2</v>
       </c>
       <c r="B2" s="6" t="n"/>
@@ -4775,7 +4206,7 @@
       <c r="J2" s="7" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="n">
+      <c r="A3" s="31" t="n">
         <v>3</v>
       </c>
       <c r="B3" s="6" t="n"/>
@@ -4817,7 +4248,7 @@
       <c r="J3" s="7" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="n">
+      <c r="A4" s="31" t="n">
         <v>4</v>
       </c>
       <c r="B4" s="6" t="n"/>
@@ -4859,7 +4290,7 @@
       <c r="J4" s="7" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="n">
+      <c r="A5" s="31" t="n">
         <v>5</v>
       </c>
       <c r="B5" s="6" t="n"/>
@@ -4901,7 +4332,7 @@
       <c r="J5" s="7" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="5" t="n">
+      <c r="A6" s="31" t="n">
         <v>6</v>
       </c>
       <c r="B6" s="6" t="n"/>
@@ -4943,7 +4374,7 @@
       <c r="J6" s="7" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" s="5" t="n">
+      <c r="A7" s="31" t="n">
         <v>7</v>
       </c>
       <c r="B7" s="6" t="n"/>
@@ -4985,7 +4416,7 @@
       <c r="J7" s="7" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="5" t="n">
+      <c r="A8" s="31" t="n">
         <v>8</v>
       </c>
       <c r="B8" s="6" t="n"/>
@@ -5027,7 +4458,7 @@
       <c r="J8" s="7" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="5" t="n">
+      <c r="A9" s="31" t="n">
         <v>9</v>
       </c>
       <c r="B9" s="6" t="n"/>
@@ -5069,7 +4500,7 @@
       <c r="J9" s="7" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" s="5" t="n">
+      <c r="A10" s="31" t="n">
         <v>10</v>
       </c>
       <c r="B10" s="6" t="n"/>
@@ -5111,7 +4542,7 @@
       <c r="J10" s="7" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="5" t="n">
+      <c r="A11" s="31" t="n">
         <v>11</v>
       </c>
       <c r="B11" s="6" t="n"/>
@@ -5153,7 +4584,7 @@
       <c r="J11" s="7" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" s="5" t="n">
+      <c r="A12" s="31" t="n">
         <v>12</v>
       </c>
       <c r="B12" s="6" t="n"/>
@@ -5195,7 +4626,7 @@
       <c r="J12" s="7" t="n"/>
     </row>
     <row r="13">
-      <c r="A13" s="5" t="n">
+      <c r="A13" s="31" t="n">
         <v>13</v>
       </c>
       <c r="B13" s="6" t="n"/>
@@ -5237,7 +4668,7 @@
       <c r="J13" s="7" t="n"/>
     </row>
     <row r="14">
-      <c r="A14" s="5" t="n">
+      <c r="A14" s="31" t="n">
         <v>14</v>
       </c>
       <c r="B14" s="6" t="n"/>
@@ -5279,7 +4710,7 @@
       <c r="J14" s="7" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" s="5" t="n">
+      <c r="A15" s="31" t="n">
         <v>15</v>
       </c>
       <c r="B15" s="6" t="n"/>
@@ -5321,7 +4752,7 @@
       <c r="J15" s="7" t="n"/>
     </row>
     <row r="16">
-      <c r="A16" s="5" t="n">
+      <c r="A16" s="31" t="n">
         <v>16</v>
       </c>
       <c r="B16" s="6" t="n"/>
@@ -5363,7 +4794,7 @@
       <c r="J16" s="7" t="n"/>
     </row>
     <row r="17">
-      <c r="A17" s="5" t="n">
+      <c r="A17" s="31" t="n">
         <v>17</v>
       </c>
       <c r="B17" s="6" t="n"/>
@@ -5405,7 +4836,7 @@
       <c r="J17" s="7" t="n"/>
     </row>
     <row r="18">
-      <c r="A18" s="5" t="n">
+      <c r="A18" s="31" t="n">
         <v>18</v>
       </c>
       <c r="B18" s="6" t="n"/>
@@ -5447,7 +4878,7 @@
       <c r="J18" s="7" t="n"/>
     </row>
     <row r="19">
-      <c r="A19" s="5" t="n">
+      <c r="A19" s="31" t="n">
         <v>19</v>
       </c>
       <c r="B19" s="6" t="n"/>
@@ -5489,7 +4920,7 @@
       <c r="J19" s="7" t="n"/>
     </row>
     <row r="20">
-      <c r="A20" s="5" t="n">
+      <c r="A20" s="31" t="n">
         <v>20</v>
       </c>
       <c r="B20" s="6" t="n"/>
@@ -5531,7 +4962,7 @@
       <c r="J20" s="7" t="n"/>
     </row>
     <row r="21">
-      <c r="A21" s="5" t="n">
+      <c r="A21" s="31" t="n">
         <v>21</v>
       </c>
       <c r="B21" s="10" t="n"/>
@@ -5573,7 +5004,7 @@
       <c r="J21" s="7" t="n"/>
     </row>
     <row r="22">
-      <c r="A22" s="5" t="n">
+      <c r="A22" s="31" t="n">
         <v>22</v>
       </c>
       <c r="B22" s="7" t="inlineStr">
@@ -5619,7 +5050,7 @@
       <c r="J22" s="7" t="n"/>
     </row>
     <row r="23">
-      <c r="A23" s="5" t="n"/>
+      <c r="A23" s="31" t="n"/>
       <c r="B23" s="10" t="n"/>
       <c r="C23" s="7" t="n"/>
       <c r="D23" s="7" t="n"/>
@@ -5631,7 +5062,7 @@
       <c r="J23" s="15" t="n"/>
     </row>
     <row r="24">
-      <c r="A24" s="5" t="n"/>
+      <c r="A24" s="31" t="n"/>
       <c r="B24" s="7" t="n"/>
       <c r="C24" s="7" t="n"/>
       <c r="D24" s="7" t="n"/>
@@ -5643,10 +5074,10 @@
       <c r="J24" s="15" t="n"/>
     </row>
     <row r="25">
-      <c r="A25" s="5" t="n">
+      <c r="A25" s="31" t="n">
         <v>11</v>
       </c>
-      <c r="B25" s="11" t="n"/>
+      <c r="B25" s="32" t="n"/>
       <c r="C25" s="7" t="inlineStr">
         <is>
           <t>发送成功-短信模板非String类型</t>
@@ -5684,10 +5115,10 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="5" t="n">
+      <c r="A26" s="31" t="n">
         <v>12</v>
       </c>
-      <c r="B26" s="12" t="n"/>
+      <c r="B26" s="33" t="n"/>
       <c r="C26" s="7" t="inlineStr">
         <is>
           <t>发送失败-手机号码非String类型</t>
@@ -5724,11 +5155,11 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="14.25" r="28" s="1">
-      <c r="A28" s="5" t="n">
+    <row customHeight="1" ht="14.25" r="28" s="36">
+      <c r="A28" s="31" t="n">
         <v>27</v>
       </c>
-      <c r="B28" s="5" t="inlineStr">
+      <c r="B28" s="31" t="inlineStr">
         <is>
           <t>账户未实名认证</t>
         </is>

</xml_diff>

<commit_message>
version 1.1 add send mail for html report
</commit_message>
<xml_diff>
--- a/data/testcases.xlsx
+++ b/data/testcases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView activeTab="3" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="7935" windowWidth="20400" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="sendMCode" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="userRegister" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="verifyUserAuth" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="bindBankCard" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sendMCode" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="userRegister" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="verifyUserAuth" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="bindBankCard" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="125725" fullCalcOnLoad="1"/>

</xml_diff>